<commit_message>
Technical note summarising work to date, some reorganisation.
</commit_message>
<xml_diff>
--- a/Design/Final/Documentation/BillOfMaterials/Manufacturing BOM - Basic model.xlsx
+++ b/Design/Final/Documentation/BillOfMaterials/Manufacturing BOM - Basic model.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$I$24</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,9 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
-  <si>
-    <t xml:space="preserve">MANUFACTURING BOM – Prototype as built</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
+  <si>
+    <t xml:space="preserve">MANUFACTURING BOM – Basic model</t>
   </si>
   <si>
     <t xml:space="preserve">ITEM</t>
@@ -115,88 +118,85 @@
     <t xml:space="preserve">018F6701</t>
   </si>
   <si>
-    <t xml:space="preserve">22mm hose fitting (hospital fittings)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PVC-30-1016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEPA filter material Grade …?</t>
+    <t xml:space="preserve">Large particle filter</t>
   </si>
   <si>
     <t xml:space="preserve">8-16/9W4P</t>
   </si>
   <si>
-    <t xml:space="preserve">O2 Sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AFR722-EE26</t>
+    <t xml:space="preserve">Temp/Humidity sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DHT12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaycar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic supplies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital barometric pressure sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMP180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi 3B+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3B+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi shield and ADC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XC9050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi GPIO expansion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XC9040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relay board 4 ch 12v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XC4419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS with battery SLA 12v 6Ah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SB2485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC-DC voltage regulator (variable)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XC4514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuelmiser Air Flow Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDO - CAF034</t>
   </si>
   <si>
     <t xml:space="preserve">Repco</t>
   </si>
   <si>
-    <t xml:space="preserve">Temp/Humidity sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DHT12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jaycar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic supplies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital barometric pressure sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMP180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raspberry Pi 3B+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3B+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raspberry Pi shield and ADC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XC9050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raspberry Pi GPIO expansion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XC9040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relay board 4 ch 12v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XC4419</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Battery SLA 12v 6Ah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SB2485</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DC-DC voltage regulator (variable)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XC4514</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuelmiser Air Flow Sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VDO - CAF034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
+    <t xml:space="preserve">Automotive parts warehouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cabinet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22” toolbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bunnings</t>
   </si>
   <si>
     <t xml:space="preserve">Total cost</t>
@@ -248,24 +248,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFED1C24"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF200"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -306,9 +294,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -323,28 +315,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -353,98 +329,37 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFED1C24"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFF200"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
@@ -455,34 +370,34 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -490,7 +405,7 @@
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -505,11 +420,11 @@
       <c r="F3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="4" t="n">
         <f aca="false">E3*D3</f>
         <v>8.91</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="4" t="n">
         <f aca="false">0.6*G3</f>
         <v>5.346</v>
       </c>
@@ -521,7 +436,7 @@
       <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -536,11 +451,11 @@
       <c r="F4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="4" t="n">
         <f aca="false">E4*D4</f>
         <v>4.5</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="4" t="n">
         <f aca="false">0.6*G4</f>
         <v>2.7</v>
       </c>
@@ -552,7 +467,7 @@
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
@@ -567,11 +482,11 @@
       <c r="F5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="G5" s="4" t="n">
         <f aca="false">E5*D5</f>
         <v>5.46</v>
       </c>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="4" t="n">
         <f aca="false">0.6*G5</f>
         <v>3.276</v>
       </c>
@@ -583,7 +498,7 @@
       <c r="A6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
@@ -598,11 +513,11 @@
       <c r="F6" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="3" t="n">
+      <c r="G6" s="4" t="n">
         <f aca="false">E6*D6</f>
         <v>60.72</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="4" t="n">
         <f aca="false">0.6*G6</f>
         <v>36.432</v>
       </c>
@@ -614,7 +529,7 @@
       <c r="A7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
@@ -629,11 +544,11 @@
       <c r="F7" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="3" t="n">
+      <c r="G7" s="4" t="n">
         <f aca="false">E7*D7</f>
         <v>7.08</v>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="4" t="n">
         <f aca="false">0.6*G7</f>
         <v>4.248</v>
       </c>
@@ -642,7 +557,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="0" t="s">
@@ -657,11 +575,11 @@
       <c r="F8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="3" t="n">
+      <c r="G8" s="4" t="n">
         <f aca="false">E8*D8</f>
         <v>29.64</v>
       </c>
-      <c r="H8" s="3" t="n">
+      <c r="H8" s="4" t="n">
         <f aca="false">0.6*G8</f>
         <v>17.784</v>
       </c>
@@ -671,9 +589,9 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="0" t="s">
@@ -688,11 +606,11 @@
       <c r="F9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="3" t="n">
+      <c r="G9" s="4" t="n">
         <f aca="false">E9*D9</f>
         <v>72.5</v>
       </c>
-      <c r="H9" s="3" t="n">
+      <c r="H9" s="4" t="n">
         <f aca="false">0.6*G9</f>
         <v>43.5</v>
       </c>
@@ -702,9 +620,9 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -719,11 +637,11 @@
       <c r="F10" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="3" t="n">
+      <c r="G10" s="4" t="n">
         <f aca="false">E10*D10</f>
         <v>72.5</v>
       </c>
-      <c r="H10" s="3" t="n">
+      <c r="H10" s="4" t="n">
         <f aca="false">0.6*G10</f>
         <v>43.5</v>
       </c>
@@ -733,9 +651,9 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -745,18 +663,18 @@
         <v>1</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>3.82</v>
+        <v>1.9</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="3" t="n">
+      <c r="G11" s="4" t="n">
         <f aca="false">E11*D11</f>
-        <v>3.82</v>
-      </c>
-      <c r="H11" s="3" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H11" s="4" t="n">
         <f aca="false">0.6*G11</f>
-        <v>2.292</v>
+        <v>1.14</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>13</v>
@@ -764,366 +682,336 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>1.9</v>
+        <v>14.9</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="G12" s="4" t="n">
         <f aca="false">E12*D12</f>
-        <v>3.8</v>
-      </c>
-      <c r="H12" s="3" t="n">
+        <v>14.9</v>
+      </c>
+      <c r="H12" s="4" t="n">
         <f aca="false">0.6*G12</f>
-        <v>2.28</v>
+        <v>8.94</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>22.9</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="G13" s="4" t="n">
+        <f aca="false">E13*D13</f>
+        <v>45.8</v>
+      </c>
+      <c r="H13" s="4" t="n">
+        <f aca="false">0.6*G13</f>
+        <v>27.48</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>93</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="3" t="n">
-        <f aca="false">E13*D13</f>
-        <v>93</v>
-      </c>
-      <c r="H13" s="3" t="n">
-        <f aca="false">0.6*G13</f>
-        <v>55.8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>38</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>65</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="4" t="n">
+        <f aca="false">E14*D14</f>
+        <v>65</v>
+      </c>
+      <c r="H14" s="4" t="n">
+        <f aca="false">0.6*G14</f>
         <v>39</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>11.9</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="3" t="n">
-        <f aca="false">E14*D14</f>
-        <v>11.9</v>
-      </c>
-      <c r="H14" s="3" t="n">
-        <f aca="false">0.6*G14</f>
-        <v>7.14</v>
-      </c>
       <c r="I14" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>43</v>
-      </c>
       <c r="D15" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>22.9</v>
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>17.9</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="G15" s="4" t="n">
         <f aca="false">E15*D15</f>
-        <v>45.8</v>
-      </c>
-      <c r="H15" s="3" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="H15" s="4" t="n">
         <f aca="false">0.6*G15</f>
-        <v>27.48</v>
+        <v>10.74</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>17.9</v>
+        <v>16.9</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="G16" s="4" t="n">
         <f aca="false">E16*D16</f>
-        <v>17.9</v>
-      </c>
-      <c r="H16" s="3" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="H16" s="4" t="n">
         <f aca="false">0.6*G16</f>
-        <v>10.74</v>
+        <v>10.14</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="5" t="n">
-        <v>99.9</v>
+      <c r="E17" s="0" t="n">
+        <v>17.9</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="G17" s="4" t="n">
         <f aca="false">E17*D17</f>
-        <v>99.9</v>
-      </c>
-      <c r="H17" s="3" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="H17" s="4" t="n">
         <f aca="false">0.6*G17</f>
-        <v>59.94</v>
+        <v>10.74</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="B18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="D18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="5" t="n">
-        <v>17.9</v>
+      <c r="E18" s="0" t="n">
+        <v>36.9</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="G18" s="4" t="n">
         <f aca="false">E18*D18</f>
-        <v>17.9</v>
-      </c>
-      <c r="H18" s="3" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="H18" s="4" t="n">
         <f aca="false">0.6*G18</f>
-        <v>10.74</v>
+        <v>22.14</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="5" t="n">
-        <v>16.9</v>
+      <c r="E19" s="0" t="n">
+        <v>10.9</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="G19" s="4" t="n">
         <f aca="false">E19*D19</f>
-        <v>16.9</v>
-      </c>
-      <c r="H19" s="3" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="H19" s="4" t="n">
         <f aca="false">0.6*G19</f>
-        <v>10.14</v>
+        <v>6.54</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="B20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>36.9</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="3" t="n">
+      <c r="G20" s="4" t="n">
         <f aca="false">E20*D20</f>
-        <v>36.9</v>
-      </c>
-      <c r="H20" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="H20" s="4" t="n">
         <f aca="false">0.6*G20</f>
-        <v>22.14</v>
+        <v>48</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>54</v>
+        <v>19</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>55</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>10.9</v>
+        <v>30</v>
       </c>
       <c r="F21" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G21" s="3" t="n">
-        <f aca="false">E21*D21</f>
-        <v>10.9</v>
-      </c>
-      <c r="H21" s="3" t="n">
+      <c r="H21" s="4" t="n">
         <f aca="false">0.6*G21</f>
-        <v>6.54</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>252.75</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G22" s="3" t="n">
-        <f aca="false">E22*D22</f>
-        <v>252.75</v>
-      </c>
-      <c r="H22" s="3" t="n">
-        <f aca="false">0.6*G22</f>
-        <v>151.65</v>
-      </c>
-      <c r="I22" s="0" t="s">
+      <c r="B22" s="6"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="10" t="n">
-        <f aca="false">SUM(G3:G22)</f>
-        <v>872.78</v>
-      </c>
-      <c r="H25" s="10" t="n">
-        <f aca="false">SUM(H3:H22)</f>
-        <v>523.668</v>
-      </c>
-    </row>
+      <c r="F23" s="2"/>
+      <c r="G23" s="7" t="n">
+        <f aca="false">SUM(G3:G21)</f>
+        <v>609.41</v>
+      </c>
+      <c r="H23" s="7" t="n">
+        <f aca="false">SUM(H3:H21)</f>
+        <v>365.646</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>